<commit_message>
23.09.25 tarihine kadar kararlaştırılmış excel dosyaları güncellendi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yeni klasör\btk42.github.io\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EARGE8PC\Desktop\btk42GithubIo\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="48">
   <si>
     <t>Sıra</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Ürün Kodu</t>
   </si>
   <si>
-    <t>Ana Grup</t>
-  </si>
-  <si>
     <t>İkincil Grup</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>AC-AKB-00-000-000-P1B1-01</t>
   </si>
   <si>
-    <t>Erişim Kontrol</t>
-  </si>
-  <si>
     <t>Akbil</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>Buzzerlı</t>
   </si>
   <si>
-    <t>İlk ürün</t>
-  </si>
-  <si>
     <t>Buton 18</t>
   </si>
   <si>
@@ -131,44 +122,64 @@
     <t>Buzzersız</t>
   </si>
   <si>
-    <t>mustafa</t>
-  </si>
-  <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>yok</t>
-  </si>
-  <si>
-    <t>13.56</t>
-  </si>
-  <si>
-    <t>https://butkon.com</t>
+    <t>AC-AKB-18-000-000-H3B1-01</t>
+  </si>
+  <si>
+    <t>AC-RFD-00-125-000-P1B1-01</t>
+  </si>
+  <si>
+    <t>AC-RFD-18-125-000-H3B1-01</t>
+  </si>
+  <si>
+    <t>AC-RFD-EK-135-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>AC-RFD-EK-135-COP-S2B1-01</t>
+  </si>
+  <si>
+    <t>AC-RFD-00-135-ANT-H4B0-01</t>
+  </si>
+  <si>
+    <t>125 KHz</t>
+  </si>
+  <si>
+    <t>AC-RFD-00-235-COP-H2B1-01</t>
+  </si>
+  <si>
+    <t>125 KHz + 13.56 MHz</t>
+  </si>
+  <si>
+    <t>AC-RFD-00-235-LOP-H2B1-01</t>
+  </si>
+  <si>
+    <t>AC-VTM-00-000-COP-H2B0-01</t>
+  </si>
+  <si>
+    <t>Vatman</t>
+  </si>
+  <si>
+    <t>AC-FRE-00-000-COP-H2B0-01</t>
+  </si>
+  <si>
+    <t>Yangın</t>
+  </si>
+  <si>
+    <t>AC-VTM-EK-000-COP-H2B0-01</t>
+  </si>
+  <si>
+    <t>Model-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -177,6 +188,39 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,7 +231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -195,18 +239,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -488,299 +563,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.21875" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="13.109375" style="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="H14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="I14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="J14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L9" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Buton Akbil url added. (AC-AKB-18-000-000-H3B1-01)
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EARGE8PC\Desktop\btk42GithubIo\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B050E054-4932-4A34-A1FF-829C24412C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <t>Sıra</t>
   </si>
@@ -168,12 +169,15 @@
   </si>
   <si>
     <t>Model-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/Button_Akbil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,11 +566,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -684,7 +688,9 @@
       <c r="J3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">

</xml_diff>

<commit_message>
Buton kartlı geçiş URL si eklendi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8207F9D8-F127-4E5A-B7EB-B7DCF090315C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8029C620-B9B2-4C94-9FBE-FF718D617158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="50">
   <si>
     <t>Sıra</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/AC-AKB-18-000-000-H3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/AC-RFD-18-125-000-H3B1-01</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -588,7 +591,7 @@
     <col min="8" max="8" width="14.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="13.109375" style="7"/>
   </cols>
   <sheetData>
@@ -759,7 +762,9 @@
       <c r="J5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -1061,9 +1066,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{F44CC468-7027-440B-A034-8DCDFD4770AE}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Eka COP Kartlı geçiş URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8029C620-B9B2-4C94-9FBE-FF718D617158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3336924-A108-4800-925A-B537007E2FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
   <si>
     <t>Sıra</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/AC-RFD-18-125-000-H3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/AC-RFD-EK-135-COP-S2B1-01</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -830,7 +833,9 @@
       <c r="J7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -1067,9 +1072,10 @@
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{F44CC468-7027-440B-A034-8DCDFD4770AE}"/>
     <hyperlink ref="K5" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
EkA RFID Anten projesinin kodu güncellendi. URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3336924-A108-4800-925A-B537007E2FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244BDEA4-3EDB-4B8D-A151-10172A1590EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="52">
   <si>
     <t>Sıra</t>
   </si>
@@ -138,9 +138,6 @@
     <t>AC-RFD-EK-135-COP-S2B1-01</t>
   </si>
   <si>
-    <t>AC-RFD-00-135-ANT-H4B0-01</t>
-  </si>
-  <si>
     <t>125 KHz</t>
   </si>
   <si>
@@ -178,6 +175,12 @@
   </si>
   <si>
     <t>https://github.com/btk42/AC-RFD-EK-135-COP-S2B1-01</t>
+  </si>
+  <si>
+    <t>AC-RFD-EK-135-ANT-H4B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/AC-RFD-EK-135-ANT-H4B0-01</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -662,7 +665,7 @@
         <v>17</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="4"/>
     </row>
@@ -695,10 +698,10 @@
         <v>17</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -730,7 +733,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="4"/>
     </row>
@@ -763,10 +766,10 @@
         <v>17</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -798,7 +801,7 @@
         <v>17</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K6" s="4"/>
     </row>
@@ -831,10 +834,10 @@
         <v>17</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -842,13 +845,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>24</v>
@@ -866,9 +869,11 @@
         <v>31</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -884,7 +889,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>14</v>
@@ -899,7 +904,7 @@
         <v>17</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -908,7 +913,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>21</v>
@@ -917,7 +922,7 @@
         <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>28</v>
@@ -932,7 +937,7 @@
         <v>17</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K10" s="4"/>
     </row>
@@ -941,7 +946,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>21</v>
@@ -950,7 +955,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>25</v>
@@ -965,7 +970,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" s="4"/>
     </row>
@@ -974,10 +979,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
@@ -998,7 +1003,7 @@
         <v>31</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="4"/>
     </row>
@@ -1007,10 +1012,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>13</v>
@@ -1031,7 +1036,7 @@
         <v>31</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K13" s="4"/>
     </row>
@@ -1040,10 +1045,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>23</v>
@@ -1064,7 +1069,7 @@
         <v>31</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" s="4"/>
     </row>
@@ -1073,9 +1078,10 @@
     <hyperlink ref="K3" r:id="rId1" xr:uid="{F44CC468-7027-440B-A034-8DCDFD4770AE}"/>
     <hyperlink ref="K5" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
     <hyperlink ref="K7" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
+    <hyperlink ref="K8" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
EKA LOP Kartlı geçiş URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244BDEA4-3EDB-4B8D-A151-10172A1590EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC14D7B0-8CA9-4D71-8747-719B6D4590A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
   <si>
     <t>Sıra</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/AC-RFD-EK-135-ANT-H4B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/AC-RFD-EK-135-LOP-S2B1-01</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -803,7 +806,9 @@
       <c r="J6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1079,9 +1084,10 @@
     <hyperlink ref="K5" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
     <hyperlink ref="K7" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
     <hyperlink ref="K8" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{332216FC-1BAF-4F1E-A717-D17B15695E41}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
ESP32 kartlı geçiş URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC14D7B0-8CA9-4D71-8747-719B6D4590A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFE5090-753F-4E93-81DA-BEE8A4A46534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
   <si>
     <t>Sıra</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/AC-RFD-EK-135-LOP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/AC-RFD-00-125-000-P1B1-01</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -738,7 +741,9 @@
       <c r="J4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -1085,9 +1090,10 @@
     <hyperlink ref="K7" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
     <hyperlink ref="K8" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
     <hyperlink ref="K6" r:id="rId5" xr:uid="{332216FC-1BAF-4F1E-A717-D17B15695E41}"/>
+    <hyperlink ref="K4" r:id="rId6" xr:uid="{CCA9C7D0-132D-4DC4-95A3-4C298D42061F}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Multi RFID Kartlı geçiş projesinin kodu güncellendi URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFE5090-753F-4E93-81DA-BEE8A4A46534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B75F98B-53B2-4E26-806B-18BF0E3F1052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
   <si>
     <t>Sıra</t>
   </si>
@@ -141,15 +141,9 @@
     <t>125 KHz</t>
   </si>
   <si>
-    <t>AC-RFD-00-235-COP-H2B1-01</t>
-  </si>
-  <si>
     <t>125 KHz + 13.56 MHz</t>
   </si>
   <si>
-    <t>AC-RFD-00-235-LOP-H2B1-01</t>
-  </si>
-  <si>
     <t>AC-VTM-00-000-COP-H2B0-01</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>https://github.com/btk42/AC-RFD-00-125-000-P1B1-01</t>
+  </si>
+  <si>
+    <t>AC-RFD-00-235-000-H3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/AC-RFD-00-235-000-H3B1-01</t>
   </si>
 </sst>
 </file>
@@ -585,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
         <v>17</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K2" s="4"/>
     </row>
@@ -704,10 +704,10 @@
         <v>17</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -739,10 +739,10 @@
         <v>17</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -774,10 +774,10 @@
         <v>17</v>
       </c>
       <c r="J5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -809,10 +809,10 @@
         <v>17</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -844,10 +844,10 @@
         <v>17</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>21</v>
@@ -879,10 +879,10 @@
         <v>31</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
         <v>17</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -923,7 +923,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>21</v>
@@ -932,43 +932,45 @@
         <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
@@ -977,10 +979,10 @@
         <v>27</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K11" s="4"/>
     </row>
@@ -1013,7 +1015,7 @@
         <v>31</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K12" s="4"/>
     </row>
@@ -1025,10 +1027,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>13</v>
@@ -1046,42 +1048,9 @@
         <v>31</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1091,9 +1060,10 @@
     <hyperlink ref="K8" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
     <hyperlink ref="K6" r:id="rId5" xr:uid="{332216FC-1BAF-4F1E-A717-D17B15695E41}"/>
     <hyperlink ref="K4" r:id="rId6" xr:uid="{CCA9C7D0-132D-4DC4-95A3-4C298D42061F}"/>
+    <hyperlink ref="K10" r:id="rId7" xr:uid="{9443A7CF-356A-4DF0-9FEE-22A2723C4A63}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Aynı proje kodları silindi. Erişim kontrol için.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B75F98B-53B2-4E26-806B-18BF0E3F1052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA90D71-9C4A-494B-9D32-02BEA0AF0EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="53">
   <si>
     <t>Sıra</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>AC-AKB-00-000-000-P1B1-01</t>
   </si>
   <si>
     <t>Akbil</t>
@@ -588,7 +585,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -647,33 +644,35 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -683,31 +682,31 @@
         <v>32</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="H3" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -718,31 +717,31 @@
         <v>33</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -753,31 +752,31 @@
         <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -788,31 +787,31 @@
         <v>35</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -820,34 +819,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -855,134 +854,132 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>49</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>53</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" s="4"/>
     </row>
@@ -991,76 +988,46 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K13" s="4"/>
+      <c r="A13" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{F44CC468-7027-440B-A034-8DCDFD4770AE}"/>
-    <hyperlink ref="K5" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
-    <hyperlink ref="K7" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
-    <hyperlink ref="K8" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
-    <hyperlink ref="K6" r:id="rId5" xr:uid="{332216FC-1BAF-4F1E-A717-D17B15695E41}"/>
-    <hyperlink ref="K4" r:id="rId6" xr:uid="{CCA9C7D0-132D-4DC4-95A3-4C298D42061F}"/>
-    <hyperlink ref="K10" r:id="rId7" xr:uid="{9443A7CF-356A-4DF0-9FEE-22A2723C4A63}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{F44CC468-7027-440B-A034-8DCDFD4770AE}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
+    <hyperlink ref="K6" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
+    <hyperlink ref="K7" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
+    <hyperlink ref="K5" r:id="rId5" xr:uid="{332216FC-1BAF-4F1E-A717-D17B15695E41}"/>
+    <hyperlink ref="K3" r:id="rId6" xr:uid="{CCA9C7D0-132D-4DC4-95A3-4C298D42061F}"/>
+    <hyperlink ref="K9" r:id="rId7" xr:uid="{9443A7CF-356A-4DF0-9FEE-22A2723C4A63}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>

<commit_message>
Bir önceki commit düzeltildi.
</commit_message>
<xml_diff>
--- a/pages/erisim-kontrol.xlsx
+++ b/pages/erisim-kontrol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA90D71-9C4A-494B-9D32-02BEA0AF0EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC68409-8F18-4287-8C91-3C8AD03FA4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,6 @@
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterate="1"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -135,9 +130,6 @@
     <t>AC-RFD-EK-135-COP-S2B1-01</t>
   </si>
   <si>
-    <t>125 KHz</t>
-  </si>
-  <si>
     <t>125 KHz + 13.56 MHz</t>
   </si>
   <si>
@@ -184,13 +176,16 @@
   </si>
   <si>
     <t>https://github.com/btk42/AC-RFD-00-235-000-H3B1-01</t>
+  </si>
+  <si>
+    <t>AC-AKB-00-000-000-P1B1-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,15 +219,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -275,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -292,14 +278,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -582,26 +571,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="13.109375" style="7"/>
+    <col min="1" max="1" width="4.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="13.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -640,73 +629,71 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="G2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="J2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -714,13 +701,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>21</v>
@@ -729,19 +716,19 @@
         <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -749,34 +736,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>20</v>
@@ -796,7 +783,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>25</v>
@@ -808,10 +795,10 @@
         <v>16</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>20</v>
@@ -831,22 +818,22 @@
         <v>23</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -854,40 +841,42 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>20</v>
@@ -896,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -911,10 +900,10 @@
         <v>16</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -922,10 +911,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -946,7 +935,7 @@
         <v>30</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K10" s="4"/>
     </row>
@@ -955,10 +944,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
@@ -979,7 +968,7 @@
         <v>30</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K11" s="4"/>
     </row>
@@ -988,10 +977,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>22</v>
@@ -1012,21 +1001,18 @@
         <v>30</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{F44CC468-7027-440B-A034-8DCDFD4770AE}"/>
-    <hyperlink ref="K4" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
-    <hyperlink ref="K6" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
-    <hyperlink ref="K7" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
-    <hyperlink ref="K5" r:id="rId5" xr:uid="{332216FC-1BAF-4F1E-A717-D17B15695E41}"/>
-    <hyperlink ref="K3" r:id="rId6" xr:uid="{CCA9C7D0-132D-4DC4-95A3-4C298D42061F}"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{F44CC468-7027-440B-A034-8DCDFD4770AE}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{60B771AF-F792-42A6-9FB1-F44C4022B9E3}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{50EEA9AE-C4B4-431E-A9A0-63C4DE0A723C}"/>
+    <hyperlink ref="K8" r:id="rId4" xr:uid="{A20537DC-BB8D-4AC6-89C3-AB406E802284}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{332216FC-1BAF-4F1E-A717-D17B15695E41}"/>
+    <hyperlink ref="K4" r:id="rId6" xr:uid="{CCA9C7D0-132D-4DC4-95A3-4C298D42061F}"/>
     <hyperlink ref="K9" r:id="rId7" xr:uid="{9443A7CF-356A-4DF0-9FEE-22A2723C4A63}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>